<commit_message>
Updating Data Dictionary tab
</commit_message>
<xml_diff>
--- a/data/combined_state_demo_data_2016_2022.xlsx
+++ b/data/combined_state_demo_data_2016_2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liam McMahon\Desktop\General Assembly\Data Science Immersive\dsb-826\Projects\youth_crime_group_project - Copy\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liam McMahon\Desktop\General Assembly\Data Science Immersive\dsb-826\Projects\project-4\data\2016-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74389A66-79CE-4A98-BDB4-0E9989B16B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2B3468-0C5E-45C2-B975-FA59228E28C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{D1250671-9D55-4F94-A1F9-874AE8287DF1}"/>
+    <workbookView xWindow="17850" yWindow="5025" windowWidth="13785" windowHeight="6000" xr2:uid="{D1250671-9D55-4F94-A1F9-874AE8287DF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="105">
   <si>
     <t>state</t>
   </si>
@@ -314,6 +314,33 @@
   </si>
   <si>
     <t>https://wonder.cdc.gov/wonder/help/mcd-expanded.html</t>
+  </si>
+  <si>
+    <t>Persons Unemployed 15 Weeks or Longer, as a Percent of the Civilian Labor Force, 4-Quarter Moving Average, Not Seasonally Adjusted</t>
+  </si>
+  <si>
+    <t>Unemployment Rate Percent, Seasonally Adjusted</t>
+  </si>
+  <si>
+    <t>U.S. Bureau of Labor Statistics, Persons Unemployed 15 Weeks or Longer, as a Percent of the Civilian Labor Force for Alabama [U1UNEM1AL], retrieved from FRED, Federal Reserve Bank of St. Louis; https://fred.stlouisfed.org/series/U1UNEM1AL, October 30, 2024.</t>
+  </si>
+  <si>
+    <t>U.S. Bureau of Labor Statistics, Unemployment Rate in Alabama [ALUR], retrieved from FRED, Federal Reserve Bank of St. Louis; https://fred.stlouisfed.org/series/ALUR, October 30, 2024.</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/U1UNEM1AL</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/ALUR</t>
+  </si>
+  <si>
+    <t>U.S. Census Bureau, Bachelor's Degree or Higher for Alabama [GCT1502AL], retrieved from FRED, Federal Reserve Bank of St. Louis; https://fred.stlouisfed.org/series/GCT1502AL, October 30, 2024.</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/GCT1502AL</t>
+  </si>
+  <si>
+    <t>Estimate of educational attainment for population 18 years old and over whose highest degree was a bachelor's, master's, or professional or doctorate degree (ACS variable S1501_C02_015E from table S1501).</t>
   </si>
 </sst>
 </file>
@@ -23016,11 +23043,29 @@
       <c r="A12" t="s">
         <v>53</v>
       </c>
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -23053,6 +23098,15 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
+      </c>
+      <c r="B16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>